<commit_message>
updated readings after h/w mods
</commit_message>
<xml_diff>
--- a/Docs/BatteryReadings.xlsx
+++ b/Docs/BatteryReadings.xlsx
@@ -15,15 +15,49 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>1 bat</t>
+  </si>
+  <si>
+    <t>0 bat</t>
+  </si>
+  <si>
+    <t>Bat1</t>
+  </si>
+  <si>
+    <t>Bat2</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>per cell</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
@@ -50,10 +84,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -92,58 +127,58 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$H$7:$H$9</c:f>
+              <c:f>Sheet1!$O$6:$O$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9.66</c:v>
+                  <c:v>11.53</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.78</c:v>
+                  <c:v>10.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.54</c:v>
+                  <c:v>10.47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$7:$I$9</c:f>
+              <c:f>Sheet1!$P$6:$P$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>686</c:v>
+                  <c:v>783</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>787</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>828</c:v>
+                  <c:v>738</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="120910592"/>
-        <c:axId val="120904704"/>
+        <c:axId val="105480576"/>
+        <c:axId val="105482112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="120910592"/>
+        <c:axId val="105480576"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120904704"/>
+        <c:crossAx val="105482112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="120904704"/>
+        <c:axId val="105482112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -151,7 +186,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120910592"/>
+        <c:crossAx val="105480576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -164,7 +199,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -490,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C3:K40"/>
+  <dimension ref="H3:Q40"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:K40"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -501,151 +536,205 @@
     <col min="10" max="10" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:11">
+    <row r="3" spans="8:17">
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>169</v>
+      </c>
       <c r="J3" s="2">
-        <f>48.947*K3+212.6</f>
-        <v>653.12300000000005</v>
+        <f>41.734*K3+302.1</f>
+        <v>677.70600000000002</v>
       </c>
       <c r="K3" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="3:11">
+    <row r="4" spans="8:17">
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>332</v>
+      </c>
       <c r="J4" s="2">
-        <f>48.947*K4+212.6</f>
-        <v>658.01769999999999</v>
+        <f t="shared" ref="J4:J40" si="0">41.734*K4+302.1</f>
+        <v>681.87940000000003</v>
       </c>
       <c r="K4" s="1">
         <v>9.1</v>
       </c>
     </row>
-    <row r="5" spans="3:11">
+    <row r="5" spans="8:17">
       <c r="J5" s="2">
-        <f t="shared" ref="J5:J40" si="0">48.947*K5+212.6</f>
-        <v>662.91239999999993</v>
+        <f t="shared" si="0"/>
+        <v>686.05279999999993</v>
       </c>
       <c r="K5" s="1">
         <v>9.1999999999999993</v>
       </c>
-    </row>
-    <row r="6" spans="3:11">
+      <c r="M5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="8:17">
       <c r="J6" s="2">
         <f t="shared" si="0"/>
-        <v>667.8071000000001</v>
+        <v>690.22620000000006</v>
       </c>
       <c r="K6" s="1">
         <v>9.3000000000000007</v>
       </c>
-    </row>
-    <row r="7" spans="3:11">
-      <c r="H7">
-        <v>9.66</v>
-      </c>
-      <c r="I7">
-        <v>686</v>
-      </c>
+      <c r="M6">
+        <v>11.53</v>
+      </c>
+      <c r="N6">
+        <v>11.75</v>
+      </c>
+      <c r="O6">
+        <f>MIN(N6,M6)</f>
+        <v>11.53</v>
+      </c>
+      <c r="P6">
+        <v>783</v>
+      </c>
+      <c r="Q6">
+        <f>O6/3</f>
+        <v>3.8433333333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="8:17">
       <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>672.70180000000005</v>
+        <v>694.39960000000008</v>
       </c>
       <c r="K7" s="1">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="8" spans="3:11">
-      <c r="H8">
-        <v>11.78</v>
-      </c>
-      <c r="I8">
-        <v>787</v>
-      </c>
+      <c r="M7">
+        <v>10.7</v>
+      </c>
+      <c r="N7">
+        <v>11.05</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ref="O7:O19" si="1">MIN(N7,M7)</f>
+        <v>10.7</v>
+      </c>
+      <c r="P7">
+        <v>750</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" ref="Q7:Q8" si="2">O7/3</f>
+        <v>3.5666666666666664</v>
+      </c>
+    </row>
+    <row r="8" spans="8:17">
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>677.59649999999999</v>
+        <v>698.57300000000009</v>
       </c>
       <c r="K8" s="1">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="9" spans="3:11">
-      <c r="C9">
-        <v>9</v>
-      </c>
-      <c r="D9">
-        <v>654</v>
-      </c>
-      <c r="H9">
-        <v>12.54</v>
-      </c>
-      <c r="I9">
-        <v>828</v>
-      </c>
+      <c r="M8" s="3">
+        <v>10.47</v>
+      </c>
+      <c r="N8" s="3">
+        <v>10.82</v>
+      </c>
+      <c r="O8" s="3">
+        <f t="shared" si="1"/>
+        <v>10.47</v>
+      </c>
+      <c r="P8" s="3">
+        <v>738</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="2"/>
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="9" spans="8:17">
       <c r="J9" s="2">
         <f t="shared" si="0"/>
-        <v>682.49120000000005</v>
+        <v>702.74639999999999</v>
       </c>
       <c r="K9" s="1">
         <v>9.6</v>
       </c>
     </row>
-    <row r="10" spans="3:11">
+    <row r="10" spans="8:17">
       <c r="J10" s="2">
         <f t="shared" si="0"/>
-        <v>687.38589999999999</v>
+        <v>706.91980000000001</v>
       </c>
       <c r="K10" s="1">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="11" spans="3:11">
+    <row r="11" spans="8:17">
       <c r="J11" s="2">
         <f t="shared" si="0"/>
-        <v>692.28060000000005</v>
+        <v>711.09320000000002</v>
       </c>
       <c r="K11" s="1">
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="12" spans="3:11">
+    <row r="12" spans="8:17">
       <c r="J12" s="2">
         <f t="shared" si="0"/>
-        <v>697.17529999999999</v>
+        <v>715.26660000000004</v>
       </c>
       <c r="K12" s="1">
         <v>9.9</v>
       </c>
     </row>
-    <row r="13" spans="3:11">
+    <row r="13" spans="8:17">
       <c r="J13" s="2">
         <f t="shared" si="0"/>
-        <v>702.07</v>
+        <v>719.44</v>
       </c>
       <c r="K13" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="3:11">
+    <row r="14" spans="8:17">
       <c r="J14" s="2">
         <f t="shared" si="0"/>
-        <v>706.96469999999999</v>
+        <v>723.61339999999996</v>
       </c>
       <c r="K14" s="1">
         <v>10.1</v>
       </c>
     </row>
-    <row r="15" spans="3:11">
+    <row r="15" spans="8:17">
       <c r="J15" s="2">
         <f t="shared" si="0"/>
-        <v>711.85939999999994</v>
+        <v>727.78680000000008</v>
       </c>
       <c r="K15" s="1">
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="16" spans="3:11">
+    <row r="16" spans="8:17">
       <c r="J16" s="2">
         <f t="shared" si="0"/>
-        <v>716.75410000000011</v>
+        <v>731.96019999999999</v>
       </c>
       <c r="K16" s="1">
         <v>10.3</v>
@@ -654,7 +743,7 @@
     <row r="17" spans="10:11">
       <c r="J17" s="2">
         <f t="shared" si="0"/>
-        <v>721.64880000000005</v>
+        <v>736.13360000000011</v>
       </c>
       <c r="K17" s="1">
         <v>10.4</v>
@@ -663,7 +752,7 @@
     <row r="18" spans="10:11">
       <c r="J18" s="2">
         <f t="shared" si="0"/>
-        <v>726.54350000000011</v>
+        <v>740.30700000000002</v>
       </c>
       <c r="K18" s="1">
         <v>10.5</v>
@@ -672,7 +761,7 @@
     <row r="19" spans="10:11">
       <c r="J19" s="2">
         <f t="shared" si="0"/>
-        <v>731.43820000000005</v>
+        <v>744.48040000000003</v>
       </c>
       <c r="K19" s="1">
         <v>10.6</v>
@@ -681,7 +770,7 @@
     <row r="20" spans="10:11">
       <c r="J20" s="2">
         <f t="shared" si="0"/>
-        <v>736.3329</v>
+        <v>748.65380000000005</v>
       </c>
       <c r="K20" s="1">
         <v>10.7</v>
@@ -690,7 +779,7 @@
     <row r="21" spans="10:11">
       <c r="J21" s="2">
         <f t="shared" si="0"/>
-        <v>741.22760000000005</v>
+        <v>752.82720000000006</v>
       </c>
       <c r="K21" s="1">
         <v>10.8</v>
@@ -699,7 +788,7 @@
     <row r="22" spans="10:11">
       <c r="J22" s="2">
         <f t="shared" si="0"/>
-        <v>746.12230000000011</v>
+        <v>757.00060000000008</v>
       </c>
       <c r="K22" s="1">
         <v>10.9</v>
@@ -708,7 +797,7 @@
     <row r="23" spans="10:11">
       <c r="J23" s="2">
         <f t="shared" si="0"/>
-        <v>751.01700000000005</v>
+        <v>761.17399999999998</v>
       </c>
       <c r="K23" s="1">
         <v>11</v>
@@ -717,7 +806,7 @@
     <row r="24" spans="10:11">
       <c r="J24" s="2">
         <f t="shared" si="0"/>
-        <v>755.9117</v>
+        <v>765.34740000000011</v>
       </c>
       <c r="K24" s="1">
         <v>11.1</v>
@@ -726,7 +815,7 @@
     <row r="25" spans="10:11">
       <c r="J25" s="2">
         <f t="shared" si="0"/>
-        <v>760.80640000000005</v>
+        <v>769.52080000000001</v>
       </c>
       <c r="K25" s="1">
         <v>11.2</v>
@@ -735,7 +824,7 @@
     <row r="26" spans="10:11">
       <c r="J26" s="2">
         <f t="shared" si="0"/>
-        <v>765.70110000000011</v>
+        <v>773.69420000000014</v>
       </c>
       <c r="K26" s="1">
         <v>11.3</v>
@@ -744,7 +833,7 @@
     <row r="27" spans="10:11">
       <c r="J27" s="2">
         <f t="shared" si="0"/>
-        <v>770.59580000000005</v>
+        <v>777.86760000000004</v>
       </c>
       <c r="K27" s="1">
         <v>11.4</v>
@@ -753,7 +842,7 @@
     <row r="28" spans="10:11">
       <c r="J28" s="2">
         <f t="shared" si="0"/>
-        <v>775.4905</v>
+        <v>782.04100000000005</v>
       </c>
       <c r="K28" s="1">
         <v>11.5</v>
@@ -762,7 +851,7 @@
     <row r="29" spans="10:11">
       <c r="J29" s="2">
         <f t="shared" si="0"/>
-        <v>780.38520000000005</v>
+        <v>786.21440000000007</v>
       </c>
       <c r="K29" s="1">
         <v>11.6</v>
@@ -771,7 +860,7 @@
     <row r="30" spans="10:11">
       <c r="J30" s="2">
         <f t="shared" si="0"/>
-        <v>785.2799</v>
+        <v>790.38779999999997</v>
       </c>
       <c r="K30" s="1">
         <v>11.7</v>
@@ -780,7 +869,7 @@
     <row r="31" spans="10:11">
       <c r="J31" s="2">
         <f t="shared" si="0"/>
-        <v>790.17460000000005</v>
+        <v>794.5612000000001</v>
       </c>
       <c r="K31" s="1">
         <v>11.8</v>
@@ -789,7 +878,7 @@
     <row r="32" spans="10:11">
       <c r="J32" s="2">
         <f t="shared" si="0"/>
-        <v>795.06930000000011</v>
+        <v>798.7346</v>
       </c>
       <c r="K32" s="1">
         <v>11.9</v>
@@ -798,7 +887,7 @@
     <row r="33" spans="10:11">
       <c r="J33" s="2">
         <f t="shared" si="0"/>
-        <v>799.96400000000006</v>
+        <v>802.90800000000002</v>
       </c>
       <c r="K33" s="1">
         <v>12</v>
@@ -807,7 +896,7 @@
     <row r="34" spans="10:11">
       <c r="J34" s="2">
         <f t="shared" si="0"/>
-        <v>804.8587</v>
+        <v>807.08140000000003</v>
       </c>
       <c r="K34" s="1">
         <v>12.1</v>
@@ -816,7 +905,7 @@
     <row r="35" spans="10:11">
       <c r="J35" s="2">
         <f t="shared" si="0"/>
-        <v>809.75340000000006</v>
+        <v>811.25479999999993</v>
       </c>
       <c r="K35" s="1">
         <v>12.2</v>
@@ -825,7 +914,7 @@
     <row r="36" spans="10:11">
       <c r="J36" s="2">
         <f t="shared" si="0"/>
-        <v>814.64810000000011</v>
+        <v>815.42820000000006</v>
       </c>
       <c r="K36" s="1">
         <v>12.3</v>
@@ -834,7 +923,7 @@
     <row r="37" spans="10:11">
       <c r="J37" s="2">
         <f t="shared" si="0"/>
-        <v>819.54280000000006</v>
+        <v>819.60160000000008</v>
       </c>
       <c r="K37" s="1">
         <v>12.4</v>
@@ -843,7 +932,7 @@
     <row r="38" spans="10:11">
       <c r="J38" s="2">
         <f t="shared" si="0"/>
-        <v>824.43750000000011</v>
+        <v>823.77500000000009</v>
       </c>
       <c r="K38" s="1">
         <v>12.5</v>
@@ -852,7 +941,7 @@
     <row r="39" spans="10:11">
       <c r="J39" s="2">
         <f t="shared" si="0"/>
-        <v>829.33220000000006</v>
+        <v>827.94839999999999</v>
       </c>
       <c r="K39" s="1">
         <v>12.6</v>
@@ -861,7 +950,7 @@
     <row r="40" spans="10:11">
       <c r="J40" s="2">
         <f t="shared" si="0"/>
-        <v>834.2269</v>
+        <v>832.12180000000001</v>
       </c>
       <c r="K40" s="1">
         <v>12.7</v>
@@ -869,7 +958,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>